<commit_message>
Association and layout of the power regulator mod
</commit_message>
<xml_diff>
--- a/Bench Buddy (Session 1 CE).xlsx
+++ b/Bench Buddy (Session 1 CE).xlsx
@@ -428,7 +428,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -439,6 +438,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -836,7 +838,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J33" sqref="J33"/>
+      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1"/>
@@ -887,8 +889,8 @@
       <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
       <c r="N1" s="1">
         <v>1</v>
       </c>
@@ -900,43 +902,43 @@
       </c>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="9">
         <v>2</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="10">
         <v>0.54</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="10">
         <f t="shared" ref="E2:E33" si="0">C2*D2</f>
         <v>1.08</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="10">
         <v>0.32340000000000002</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="10">
         <f t="shared" ref="G2:G33" si="1">F2*C2</f>
         <v>0.64680000000000004</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="10">
         <v>0.1862</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="10">
         <f t="shared" ref="I2:I33" si="2">H2*C2</f>
         <v>0.37240000000000001</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="L2" s="14"/>
+      <c r="K2" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L2" s="13"/>
       <c r="M2" s="1" t="s">
         <v>9</v>
       </c>
@@ -954,43 +956,43 @@
       </c>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4">
-        <v>1</v>
-      </c>
-      <c r="D3" s="7">
+      <c r="C3" s="9">
+        <v>1</v>
+      </c>
+      <c r="D3" s="10">
         <v>0.06</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="10">
         <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="10">
         <v>3.4799999999999998E-2</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="10">
         <f t="shared" si="1"/>
         <v>3.4799999999999998E-2</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="10">
         <v>1.9689999999999999E-2</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="10">
         <f t="shared" si="2"/>
         <v>1.9689999999999999E-2</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="L3" s="14"/>
+      <c r="K3" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L3" s="13"/>
       <c r="M3" s="1" t="s">
         <v>18</v>
       </c>
@@ -1008,43 +1010,43 @@
       </c>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="7">
+      <c r="C4" s="9">
+        <v>1</v>
+      </c>
+      <c r="D4" s="10">
         <v>0.31</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="10">
         <f t="shared" si="0"/>
         <v>0.31</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="10">
         <v>0.25700000000000001</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="10">
         <f t="shared" si="1"/>
         <v>0.25700000000000001</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="10">
         <v>0.17299999999999999</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="10">
         <f t="shared" si="2"/>
         <v>0.17299999999999999</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="L4" s="14"/>
+      <c r="K4" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L4" s="13"/>
       <c r="M4" s="1" t="s">
         <v>21</v>
       </c>
@@ -1062,43 +1064,43 @@
       </c>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="4">
-        <v>1</v>
-      </c>
-      <c r="D5" s="7">
+      <c r="C5" s="9">
+        <v>1</v>
+      </c>
+      <c r="D5" s="10">
         <v>1.36</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="10">
         <f t="shared" si="0"/>
         <v>1.36</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="10">
         <v>0.86</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="10">
         <f t="shared" si="1"/>
         <v>0.86</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="10">
         <v>0.86</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="10">
         <f t="shared" si="2"/>
         <v>0.86</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="L5" s="14"/>
+      <c r="K5" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L5" s="13"/>
       <c r="M5" s="1" t="s">
         <v>32</v>
       </c>
@@ -1149,10 +1151,10 @@
       <c r="J6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="L6" s="14"/>
+      <c r="K6" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L6" s="13"/>
       <c r="M6" s="1" t="s">
         <v>24</v>
       </c>
@@ -1170,43 +1172,43 @@
       </c>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="4">
-        <v>1</v>
-      </c>
-      <c r="D7" s="7">
+      <c r="C7" s="9">
+        <v>1</v>
+      </c>
+      <c r="D7" s="10">
         <v>0.5</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="10">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="10">
         <v>0.44940000000000002</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="10">
         <f t="shared" si="1"/>
         <v>0.44940000000000002</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="10">
         <v>0.35699999999999998</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="10">
         <f t="shared" si="2"/>
         <v>0.35699999999999998</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="K7" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="L7" s="14"/>
+      <c r="K7" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L7" s="13"/>
       <c r="M7" s="1" t="s">
         <v>49</v>
       </c>
@@ -1224,43 +1226,43 @@
       </c>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="4">
-        <v>1</v>
-      </c>
-      <c r="D8" s="7">
+      <c r="C8" s="9">
+        <v>1</v>
+      </c>
+      <c r="D8" s="10">
         <v>1.57</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="10">
         <f t="shared" si="0"/>
         <v>1.57</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="10">
         <v>1.22</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="10">
         <f t="shared" si="1"/>
         <v>1.22</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="10">
         <v>0.875</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="10">
         <f t="shared" si="2"/>
         <v>0.875</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="K8" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="L8" s="14"/>
+      <c r="K8" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L8" s="13"/>
       <c r="M8" s="1" t="s">
         <v>55</v>
       </c>
@@ -1278,43 +1280,43 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="12" customHeight="1">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="4">
-        <v>1</v>
-      </c>
-      <c r="D9" s="7">
+      <c r="C9" s="9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="10">
         <v>3.56</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="10">
         <f t="shared" si="0"/>
         <v>3.56</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="10">
         <v>2.4900000000000002</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="10">
         <f t="shared" si="1"/>
         <v>2.4900000000000002</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="10">
         <v>1.89</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="10">
         <f t="shared" si="2"/>
         <v>1.89</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="J9" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="K9" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="L9" s="14"/>
+      <c r="K9" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L9" s="13"/>
       <c r="M9" s="1" t="s">
         <v>66</v>
       </c>
@@ -1332,43 +1334,43 @@
       </c>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="4">
-        <v>1</v>
-      </c>
-      <c r="D10" s="7">
+      <c r="C10" s="9">
+        <v>1</v>
+      </c>
+      <c r="D10" s="10">
         <v>0.89</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="10">
         <f t="shared" si="0"/>
         <v>0.89</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="10">
         <v>0.65480000000000005</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="10">
         <f t="shared" si="1"/>
         <v>0.65480000000000005</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="10">
         <v>0.44431999999999999</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="10">
         <f t="shared" si="2"/>
         <v>0.44431999999999999</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="K10" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="L10" s="14"/>
+      <c r="K10" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L10" s="13"/>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="1" t="s">
@@ -1404,10 +1406,10 @@
       <c r="J11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="K11" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="L11" s="14"/>
+      <c r="K11" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="1" t="s">
@@ -1443,10 +1445,10 @@
       <c r="J12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="K12" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="L12" s="14"/>
+      <c r="K12" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L12" s="13"/>
       <c r="M12" s="1" t="s">
         <v>29</v>
       </c>
@@ -1497,10 +1499,10 @@
       <c r="J13" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="K13" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="L13" s="14"/>
+      <c r="K13" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="1" t="s">
@@ -1536,10 +1538,10 @@
       <c r="J14" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="K14" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="L14" s="14"/>
+      <c r="K14" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="1" t="s">
@@ -1575,10 +1577,10 @@
       <c r="J15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="K15" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="L15" s="14"/>
+      <c r="K15" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L15" s="13"/>
       <c r="M15" s="5" t="s">
         <v>69</v>
       </c>
@@ -1629,10 +1631,10 @@
       <c r="J16" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="K16" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="L16" s="14"/>
+      <c r="K16" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L16" s="13"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
@@ -1671,10 +1673,10 @@
       <c r="J17" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="K17" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="L17" s="14"/>
+      <c r="K17" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L17" s="13"/>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="1" t="s">
@@ -1710,10 +1712,10 @@
       <c r="J18" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="K18" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="L18" s="14"/>
+      <c r="K18" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L18" s="13"/>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="1" t="s">
@@ -1749,10 +1751,10 @@
       <c r="J19" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="K19" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="L19" s="14"/>
+      <c r="K19" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="1" t="s">
@@ -1788,355 +1790,355 @@
       <c r="J20" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="K20" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="L20" s="14"/>
+      <c r="K20" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L20" s="13"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="9">
         <v>4</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="10">
         <v>0.31</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="10">
         <f t="shared" si="0"/>
         <v>1.24</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="10">
         <v>0.25800000000000001</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="10">
         <f t="shared" si="1"/>
         <v>1.032</v>
       </c>
-      <c r="H21" s="7">
+      <c r="H21" s="10">
         <v>0.17299999999999999</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I21" s="10">
         <f t="shared" si="2"/>
         <v>0.69199999999999995</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="J21" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="K21" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="L21" s="14"/>
+      <c r="K21" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L21" s="13"/>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="9">
         <v>2</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="10">
         <v>0.22</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="10">
         <f t="shared" si="0"/>
         <v>0.44</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="10">
         <v>0.14399999999999999</v>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="10">
         <f t="shared" si="1"/>
         <v>0.28799999999999998</v>
       </c>
-      <c r="H22" s="7">
+      <c r="H22" s="10">
         <v>0.10199999999999999</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I22" s="10">
         <f t="shared" si="2"/>
         <v>0.20399999999999999</v>
       </c>
-      <c r="J22" s="3" t="s">
+      <c r="J22" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="K22" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="L22" s="14"/>
+      <c r="K22" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L22" s="13"/>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="4">
-        <v>1</v>
-      </c>
-      <c r="D23" s="7">
+      <c r="C23" s="9">
+        <v>1</v>
+      </c>
+      <c r="D23" s="10">
         <v>0.35</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="10">
         <f t="shared" si="0"/>
         <v>0.35</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="10">
         <v>0.28199999999999997</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="10">
         <f t="shared" si="1"/>
         <v>0.28199999999999997</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23" s="10">
         <v>0.22600000000000001</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I23" s="10">
         <f t="shared" si="2"/>
         <v>0.22600000000000001</v>
       </c>
-      <c r="J23" s="3" t="s">
+      <c r="J23" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="K23" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="L23" s="14"/>
+      <c r="K23" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L23" s="13"/>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="10">
-        <v>1</v>
-      </c>
-      <c r="D24" s="11">
+      <c r="C24" s="9">
+        <v>1</v>
+      </c>
+      <c r="D24" s="10">
         <v>1.1499999999999999</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E24" s="10">
         <f t="shared" si="0"/>
         <v>1.1499999999999999</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="10">
         <v>0.72</v>
       </c>
-      <c r="G24" s="11">
+      <c r="G24" s="10">
         <f t="shared" si="1"/>
         <v>0.72</v>
       </c>
-      <c r="H24" s="11">
+      <c r="H24" s="10">
         <v>0.57999999999999996</v>
       </c>
-      <c r="I24" s="11">
+      <c r="I24" s="10">
         <f t="shared" si="2"/>
         <v>0.57999999999999996</v>
       </c>
-      <c r="J24" s="12" t="s">
+      <c r="J24" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="K24" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="L24" s="14"/>
+      <c r="K24" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L24" s="13"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="10">
-        <v>1</v>
-      </c>
-      <c r="D25" s="11">
+      <c r="C25" s="9">
+        <v>1</v>
+      </c>
+      <c r="D25" s="10">
         <v>0.12</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E25" s="10">
         <f t="shared" si="0"/>
         <v>0.12</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F25" s="10">
         <v>7.4200000000000002E-2</v>
       </c>
-      <c r="G25" s="11">
+      <c r="G25" s="10">
         <f t="shared" si="1"/>
         <v>7.4200000000000002E-2</v>
       </c>
-      <c r="H25" s="11">
+      <c r="H25" s="10">
         <v>2.4719999999999999E-2</v>
       </c>
-      <c r="I25" s="11">
+      <c r="I25" s="10">
         <f t="shared" si="2"/>
         <v>2.4719999999999999E-2</v>
       </c>
-      <c r="J25" s="12" t="s">
+      <c r="J25" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="K25" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="L25" s="14"/>
+      <c r="K25" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L25" s="13"/>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="10">
-        <v>1</v>
-      </c>
-      <c r="D26" s="11">
+      <c r="C26" s="9">
+        <v>1</v>
+      </c>
+      <c r="D26" s="10">
         <v>0.39</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E26" s="10">
         <f t="shared" si="0"/>
         <v>0.39</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F26" s="10">
         <v>0.18140000000000001</v>
       </c>
-      <c r="G26" s="11">
+      <c r="G26" s="10">
         <f t="shared" si="1"/>
         <v>0.18140000000000001</v>
       </c>
-      <c r="H26" s="11">
+      <c r="H26" s="10">
         <v>0.10206</v>
       </c>
-      <c r="I26" s="11">
+      <c r="I26" s="10">
         <f t="shared" si="2"/>
         <v>0.10206</v>
       </c>
-      <c r="J26" s="12" t="s">
+      <c r="J26" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="K26" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="L26" s="14"/>
+      <c r="K26" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L26" s="13"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="10">
-        <v>1</v>
-      </c>
-      <c r="D27" s="11">
+      <c r="C27" s="9">
+        <v>1</v>
+      </c>
+      <c r="D27" s="10">
         <v>0.43</v>
       </c>
-      <c r="E27" s="11">
+      <c r="E27" s="10">
         <f t="shared" si="0"/>
         <v>0.43</v>
       </c>
-      <c r="F27" s="11">
+      <c r="F27" s="10">
         <v>0.1802</v>
       </c>
-      <c r="G27" s="11">
+      <c r="G27" s="10">
         <f t="shared" si="1"/>
         <v>0.1802</v>
       </c>
-      <c r="H27" s="11">
+      <c r="H27" s="10">
         <v>7.8200000000000006E-2</v>
       </c>
-      <c r="I27" s="11">
+      <c r="I27" s="10">
         <f t="shared" si="2"/>
         <v>7.8200000000000006E-2</v>
       </c>
-      <c r="J27" s="12" t="s">
+      <c r="J27" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="K27" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="L27" s="14"/>
+      <c r="K27" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L27" s="13"/>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="8" t="s">
         <v>55</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C28" s="4">
-        <v>1</v>
-      </c>
-      <c r="D28" s="7">
+      <c r="C28" s="9">
+        <v>1</v>
+      </c>
+      <c r="D28" s="10">
         <v>0.08</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="10">
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="10">
         <v>5.4600000000000003E-2</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G28" s="10">
         <f t="shared" si="1"/>
         <v>5.4600000000000003E-2</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H28" s="10">
         <v>0.04</v>
       </c>
-      <c r="I28" s="7">
+      <c r="I28" s="10">
         <f t="shared" si="2"/>
         <v>0.04</v>
       </c>
-      <c r="J28" s="3" t="s">
+      <c r="J28" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="K28" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="L28" s="14"/>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="1" t="s">
+      <c r="K28" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L28" s="13"/>
+    </row>
+    <row r="29" spans="1:12" s="8" customFormat="1">
+      <c r="A29" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C29" s="4">
-        <v>1</v>
-      </c>
-      <c r="D29" s="7">
+      <c r="C29" s="9">
+        <v>1</v>
+      </c>
+      <c r="D29" s="10">
         <v>2.39</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="10">
         <f t="shared" si="0"/>
         <v>2.39</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="10">
         <v>1.51</v>
       </c>
-      <c r="G29" s="7">
+      <c r="G29" s="10">
         <f t="shared" si="1"/>
         <v>1.51</v>
       </c>
-      <c r="H29" s="7">
+      <c r="H29" s="10">
         <v>1.51</v>
       </c>
-      <c r="I29" s="7">
+      <c r="I29" s="10">
         <f t="shared" si="2"/>
         <v>1.51</v>
       </c>
-      <c r="J29" s="3" t="s">
+      <c r="J29" s="11" t="s">
         <v>68</v>
       </c>
       <c r="K29" s="14" t="s">
@@ -2144,38 +2146,38 @@
       </c>
       <c r="L29" s="14"/>
     </row>
-    <row r="30" spans="1:12">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:12" s="8" customFormat="1">
+      <c r="A30" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="4">
-        <v>1</v>
-      </c>
-      <c r="D30" s="7">
+      <c r="C30" s="9">
+        <v>1</v>
+      </c>
+      <c r="D30" s="10">
         <v>2.58</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="10">
         <f t="shared" si="0"/>
         <v>2.58</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="10">
         <v>1.87</v>
       </c>
-      <c r="G30" s="7">
+      <c r="G30" s="10">
         <f t="shared" si="1"/>
         <v>1.87</v>
       </c>
-      <c r="H30" s="7">
+      <c r="H30" s="10">
         <v>1.32</v>
       </c>
-      <c r="I30" s="7">
+      <c r="I30" s="10">
         <f t="shared" si="2"/>
         <v>1.32</v>
       </c>
-      <c r="J30" s="3" t="s">
+      <c r="J30" s="11" t="s">
         <v>71</v>
       </c>
       <c r="K30" s="14" t="s">
@@ -2183,38 +2185,38 @@
       </c>
       <c r="L30" s="14"/>
     </row>
-    <row r="31" spans="1:12">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:12" s="8" customFormat="1">
+      <c r="A31" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="4">
-        <v>1</v>
-      </c>
-      <c r="D31" s="7">
+      <c r="C31" s="9">
+        <v>1</v>
+      </c>
+      <c r="D31" s="10">
         <v>0.73</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="10">
         <f t="shared" si="0"/>
         <v>0.73</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="10">
         <v>0.23760000000000001</v>
       </c>
-      <c r="G31" s="7">
+      <c r="G31" s="10">
         <f t="shared" si="1"/>
         <v>0.23760000000000001</v>
       </c>
-      <c r="H31" s="7">
+      <c r="H31" s="10">
         <v>0.224</v>
       </c>
-      <c r="I31" s="7">
+      <c r="I31" s="10">
         <f t="shared" si="2"/>
         <v>0.224</v>
       </c>
-      <c r="J31" s="3" t="s">
+      <c r="J31" s="11" t="s">
         <v>73</v>
       </c>
       <c r="K31" s="14" t="s">
@@ -2222,38 +2224,38 @@
       </c>
       <c r="L31" s="14"/>
     </row>
-    <row r="32" spans="1:12">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:12" s="8" customFormat="1">
+      <c r="A32" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="9">
         <v>4</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="10">
         <v>0.65</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="10">
         <f t="shared" si="0"/>
         <v>2.6</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="10">
         <v>0.24</v>
       </c>
-      <c r="G32" s="7">
+      <c r="G32" s="10">
         <f t="shared" si="1"/>
         <v>0.96</v>
       </c>
-      <c r="H32" s="7">
+      <c r="H32" s="10">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I32" s="7">
+      <c r="I32" s="10">
         <f t="shared" si="2"/>
         <v>0.56000000000000005</v>
       </c>
-      <c r="J32" s="3" t="s">
+      <c r="J32" s="11" t="s">
         <v>75</v>
       </c>
       <c r="K32" s="14" t="s">
@@ -2261,38 +2263,38 @@
       </c>
       <c r="L32" s="14"/>
     </row>
-    <row r="33" spans="1:12">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:12" s="8" customFormat="1">
+      <c r="A33" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="9">
         <v>3</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33" s="10">
         <v>0.1</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33" s="10">
         <f t="shared" si="0"/>
         <v>0.30000000000000004</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F33" s="10">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="G33" s="7">
+      <c r="G33" s="10">
         <f t="shared" si="1"/>
         <v>0.17400000000000002</v>
       </c>
-      <c r="H33" s="7">
+      <c r="H33" s="10">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="I33" s="7">
+      <c r="I33" s="10">
         <f t="shared" si="2"/>
         <v>0.126</v>
       </c>
-      <c r="J33" s="3" t="s">
+      <c r="J33" s="11" t="s">
         <v>77</v>
       </c>
       <c r="K33" s="14" t="s">
@@ -2302,28 +2304,28 @@
     </row>
     <row r="34" spans="1:12">
       <c r="J34" s="3"/>
-      <c r="K34" s="13"/>
-      <c r="L34" s="13"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
     </row>
     <row r="35" spans="1:12">
       <c r="J35" s="3"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="12"/>
     </row>
     <row r="36" spans="1:12">
       <c r="J36" s="3"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="12"/>
     </row>
     <row r="37" spans="1:12">
       <c r="J37" s="3"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
+      <c r="K37" s="12"/>
+      <c r="L37" s="12"/>
     </row>
     <row r="38" spans="1:12">
       <c r="J38" s="3"/>
-      <c r="K38" s="13"/>
-      <c r="L38" s="13"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
     </row>
   </sheetData>
   <sortState ref="A2:J80">

</xml_diff>